<commit_message>
Ajuste parâmetros de planta
</commit_message>
<xml_diff>
--- a/R/CropModels/Soybean/Soybean_support.xlsx
+++ b/R/CropModels/Soybean/Soybean_support.xlsx
@@ -1754,9 +1754,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1773,6 +1770,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2109,10 +2109,10 @@
       <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2994,478 +2994,478 @@
       <selection sqref="A1:XFD1048576"/>
       <selection pane="topRight" sqref="A1:XFD1048576"/>
       <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
-      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="28"/>
-    <col min="2" max="2" width="20.77734375" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.77734375" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.88671875" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" style="28" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="26"/>
+    <col min="1" max="1" width="8.88671875" style="27"/>
+    <col min="2" max="2" width="20.77734375" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.88671875" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="27" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>435</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>445</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>446</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>444</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>434</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>443</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="25" t="s">
         <v>442</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>339</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>439</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>438</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>450</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>437</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>452</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>447</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>447</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>454</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="25" t="s">
         <v>453</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>458</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>459</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="30" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>456</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>448</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="30" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>241</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>475</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="25" t="s">
         <v>474</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="30" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>477</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>478</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="30" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="25" t="s">
         <v>470</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>472</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="30" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>463</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>477</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>482</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>469</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="25" t="s">
         <v>467</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>472</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="31" t="s">
         <v>481</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>468</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>472</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="30" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>464</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>466</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>465</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>484</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="30" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>485</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>500</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>507</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="30" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>233</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>498</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>500</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>499</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>501</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>503</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>502</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>477</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>504</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>486</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>506</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="25" t="s">
         <v>505</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>487</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>496</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="25" t="s">
         <v>494</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>488</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>496</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="25" t="s">
         <v>495</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="30" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>491</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="25" t="s">
         <v>490</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="30" t="s">
         <v>492</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="25" t="s">
         <v>489</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="30" t="s">
         <v>493</v>
       </c>
     </row>

</xml_diff>